<commit_message>
perbaiki tabel json lkps
</commit_message>
<xml_diff>
--- a/common/required/kriteria9/aps/template/kuantitatif.xlsx
+++ b/common/required/kriteria9/aps/template/kuantitatif.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adryanev\Code\php\kriteria\common\required\kriteria9\aps\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BC31B6-B915-43F9-9747-00FA07704367}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C392B73E-FF47-4F05-97DA-D38B6C900081}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="839" firstSheet="22" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14055" yWindow="3240" windowWidth="15840" windowHeight="11505" tabRatio="839" firstSheet="34" activeTab="47" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="68" r:id="rId1"/>
@@ -40,11 +40,11 @@
     <sheet name="4" sheetId="62" r:id="rId25"/>
     <sheet name="5a" sheetId="35" r:id="rId26"/>
     <sheet name="5b" sheetId="36" r:id="rId27"/>
-    <sheet name="6a" sheetId="38" r:id="rId28"/>
-    <sheet name="6b" sheetId="39" r:id="rId29"/>
-    <sheet name="7" sheetId="40" r:id="rId30"/>
-    <sheet name="8a" sheetId="41" r:id="rId31"/>
-    <sheet name="5c" sheetId="37" r:id="rId32"/>
+    <sheet name="5c" sheetId="37" r:id="rId28"/>
+    <sheet name="6a" sheetId="38" r:id="rId29"/>
+    <sheet name="6b" sheetId="39" r:id="rId30"/>
+    <sheet name="7" sheetId="40" r:id="rId31"/>
+    <sheet name="8a" sheetId="41" r:id="rId32"/>
     <sheet name="8b1" sheetId="42" r:id="rId33"/>
     <sheet name="8b2" sheetId="43" r:id="rId34"/>
     <sheet name="8c" sheetId="44" r:id="rId35"/>
@@ -72,10 +72,10 @@
     <definedName name="diploma" localSheetId="22">#REF!</definedName>
     <definedName name="diploma" localSheetId="23">#REF!</definedName>
     <definedName name="diploma" localSheetId="26">#REF!</definedName>
-    <definedName name="diploma" localSheetId="31">#REF!</definedName>
     <definedName name="diploma" localSheetId="27">#REF!</definedName>
     <definedName name="diploma" localSheetId="28">#REF!</definedName>
     <definedName name="diploma" localSheetId="29">#REF!</definedName>
+    <definedName name="diploma" localSheetId="30">#REF!</definedName>
     <definedName name="diploma" localSheetId="33">#REF!</definedName>
     <definedName name="diploma" localSheetId="36">#REF!</definedName>
     <definedName name="diploma" localSheetId="40">#REF!</definedName>
@@ -2810,6 +2810,15 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2825,21 +2834,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2897,12 +2897,12 @@
     <xf numFmtId="0" fontId="20" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2966,6 +2966,9 @@
     <xf numFmtId="0" fontId="20" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2980,9 +2983,6 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3526,62 +3526,62 @@
       <c r="Y1" s="2"/>
     </row>
     <row r="2" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="126"/>
-      <c r="F2" s="126"/>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="126"/>
-      <c r="M2" s="126"/>
-      <c r="N2" s="126"/>
-      <c r="O2" s="126"/>
-      <c r="P2" s="126"/>
-      <c r="Q2" s="126"/>
-      <c r="R2" s="126"/>
-      <c r="S2" s="126"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="129"/>
+      <c r="M2" s="129"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="129"/>
+      <c r="P2" s="129"/>
+      <c r="Q2" s="129"/>
+      <c r="R2" s="129"/>
+      <c r="S2" s="129"/>
+      <c r="T2" s="129"/>
+      <c r="U2" s="129"/>
+      <c r="V2" s="129"/>
+      <c r="W2" s="129"/>
+      <c r="X2" s="129"/>
+      <c r="Y2" s="129"/>
     </row>
     <row r="3" spans="1:25" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="127" t="s">
+      <c r="A3" s="130" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="127"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="127"/>
-      <c r="G3" s="127"/>
-      <c r="H3" s="127"/>
-      <c r="I3" s="127"/>
-      <c r="J3" s="127"/>
-      <c r="K3" s="127"/>
-      <c r="L3" s="127"/>
-      <c r="M3" s="127"/>
-      <c r="N3" s="127"/>
-      <c r="O3" s="127"/>
-      <c r="P3" s="127"/>
-      <c r="Q3" s="127"/>
-      <c r="R3" s="127"/>
-      <c r="S3" s="127"/>
-      <c r="T3" s="127"/>
-      <c r="U3" s="127"/>
-      <c r="V3" s="127"/>
-      <c r="W3" s="127"/>
-      <c r="X3" s="127"/>
-      <c r="Y3" s="127"/>
+      <c r="B3" s="130"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="130"/>
+      <c r="N3" s="130"/>
+      <c r="O3" s="130"/>
+      <c r="P3" s="130"/>
+      <c r="Q3" s="130"/>
+      <c r="R3" s="130"/>
+      <c r="S3" s="130"/>
+      <c r="T3" s="130"/>
+      <c r="U3" s="130"/>
+      <c r="V3" s="130"/>
+      <c r="W3" s="130"/>
+      <c r="X3" s="130"/>
+      <c r="Y3" s="130"/>
     </row>
     <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
@@ -3622,23 +3622,23 @@
       <c r="G5" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H5" s="128"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="128"/>
-      <c r="K5" s="128"/>
-      <c r="L5" s="128"/>
-      <c r="M5" s="128"/>
-      <c r="N5" s="128"/>
-      <c r="O5" s="128"/>
-      <c r="P5" s="128"/>
-      <c r="Q5" s="128"/>
-      <c r="R5" s="128"/>
-      <c r="S5" s="128"/>
-      <c r="T5" s="128"/>
-      <c r="U5" s="128"/>
-      <c r="V5" s="128"/>
-      <c r="W5" s="128"/>
-      <c r="X5" s="128"/>
+      <c r="H5" s="131"/>
+      <c r="I5" s="131"/>
+      <c r="J5" s="131"/>
+      <c r="K5" s="131"/>
+      <c r="L5" s="131"/>
+      <c r="M5" s="131"/>
+      <c r="N5" s="131"/>
+      <c r="O5" s="131"/>
+      <c r="P5" s="131"/>
+      <c r="Q5" s="131"/>
+      <c r="R5" s="131"/>
+      <c r="S5" s="131"/>
+      <c r="T5" s="131"/>
+      <c r="U5" s="131"/>
+      <c r="V5" s="131"/>
+      <c r="W5" s="131"/>
+      <c r="X5" s="131"/>
       <c r="Y5" s="9"/>
     </row>
     <row r="6" spans="1:25" s="7" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
@@ -3680,13 +3680,13 @@
       <c r="G7" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="129"/>
-      <c r="I7" s="129"/>
-      <c r="J7" s="129"/>
-      <c r="K7" s="129"/>
-      <c r="L7" s="129"/>
-      <c r="M7" s="129"/>
-      <c r="N7" s="129"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="125"/>
+      <c r="J7" s="125"/>
+      <c r="K7" s="125"/>
+      <c r="L7" s="125"/>
+      <c r="M7" s="125"/>
+      <c r="N7" s="125"/>
       <c r="O7" s="11"/>
       <c r="P7" s="11"/>
       <c r="Q7" s="11"/>
@@ -3968,9 +3968,9 @@
       <c r="G17" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H17" s="129"/>
-      <c r="I17" s="129"/>
-      <c r="J17" s="129"/>
+      <c r="H17" s="125"/>
+      <c r="I17" s="125"/>
+      <c r="J17" s="125"/>
       <c r="K17" s="11" t="str">
         <f>IF(H17="Minimum","Studi telah mendapt ijin pembukaan program studi baru. Pengajuan usulan akreditasi pertama","")</f>
         <v/>
@@ -4259,13 +4259,13 @@
       <c r="G27" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H27" s="129"/>
-      <c r="I27" s="129"/>
-      <c r="J27" s="129"/>
-      <c r="K27" s="129"/>
-      <c r="L27" s="129"/>
-      <c r="M27" s="129"/>
-      <c r="N27" s="129"/>
+      <c r="H27" s="125"/>
+      <c r="I27" s="125"/>
+      <c r="J27" s="125"/>
+      <c r="K27" s="125"/>
+      <c r="L27" s="125"/>
+      <c r="M27" s="125"/>
+      <c r="N27" s="125"/>
       <c r="O27" s="11"/>
       <c r="P27" s="11"/>
       <c r="Q27" s="11"/>
@@ -4317,9 +4317,9 @@
       <c r="G29" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H29" s="130"/>
-      <c r="I29" s="130"/>
-      <c r="J29" s="130"/>
+      <c r="H29" s="132"/>
+      <c r="I29" s="132"/>
+      <c r="J29" s="132"/>
       <c r="K29" s="11"/>
       <c r="L29" s="11"/>
       <c r="M29" s="11"/>
@@ -4375,23 +4375,23 @@
       <c r="G31" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H31" s="128"/>
-      <c r="I31" s="128"/>
-      <c r="J31" s="128"/>
-      <c r="K31" s="128"/>
-      <c r="L31" s="128"/>
-      <c r="M31" s="128"/>
-      <c r="N31" s="128"/>
-      <c r="O31" s="128"/>
-      <c r="P31" s="128"/>
-      <c r="Q31" s="128"/>
-      <c r="R31" s="128"/>
-      <c r="S31" s="128"/>
-      <c r="T31" s="128"/>
-      <c r="U31" s="128"/>
-      <c r="V31" s="128"/>
-      <c r="W31" s="128"/>
-      <c r="X31" s="128"/>
+      <c r="H31" s="131"/>
+      <c r="I31" s="131"/>
+      <c r="J31" s="131"/>
+      <c r="K31" s="131"/>
+      <c r="L31" s="131"/>
+      <c r="M31" s="131"/>
+      <c r="N31" s="131"/>
+      <c r="O31" s="131"/>
+      <c r="P31" s="131"/>
+      <c r="Q31" s="131"/>
+      <c r="R31" s="131"/>
+      <c r="S31" s="131"/>
+      <c r="T31" s="131"/>
+      <c r="U31" s="131"/>
+      <c r="V31" s="131"/>
+      <c r="W31" s="131"/>
+      <c r="X31" s="131"/>
       <c r="Y31" s="9"/>
     </row>
     <row r="32" spans="1:25" s="7" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4433,23 +4433,23 @@
       <c r="G33" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H33" s="131"/>
-      <c r="I33" s="131"/>
-      <c r="J33" s="131"/>
-      <c r="K33" s="131"/>
-      <c r="L33" s="131"/>
-      <c r="M33" s="131"/>
-      <c r="N33" s="131"/>
-      <c r="O33" s="131"/>
-      <c r="P33" s="131"/>
-      <c r="Q33" s="131"/>
-      <c r="R33" s="131"/>
-      <c r="S33" s="131"/>
-      <c r="T33" s="131"/>
-      <c r="U33" s="131"/>
-      <c r="V33" s="131"/>
-      <c r="W33" s="131"/>
-      <c r="X33" s="131"/>
+      <c r="H33" s="133"/>
+      <c r="I33" s="133"/>
+      <c r="J33" s="133"/>
+      <c r="K33" s="133"/>
+      <c r="L33" s="133"/>
+      <c r="M33" s="133"/>
+      <c r="N33" s="133"/>
+      <c r="O33" s="133"/>
+      <c r="P33" s="133"/>
+      <c r="Q33" s="133"/>
+      <c r="R33" s="133"/>
+      <c r="S33" s="133"/>
+      <c r="T33" s="133"/>
+      <c r="U33" s="133"/>
+      <c r="V33" s="133"/>
+      <c r="W33" s="133"/>
+      <c r="X33" s="133"/>
       <c r="Y33" s="9"/>
     </row>
     <row r="34" spans="1:25" s="7" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4661,23 +4661,23 @@
       <c r="G41" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H41" s="129"/>
-      <c r="I41" s="129"/>
-      <c r="J41" s="129"/>
-      <c r="K41" s="129"/>
-      <c r="L41" s="129"/>
-      <c r="M41" s="129"/>
-      <c r="N41" s="129"/>
-      <c r="O41" s="129"/>
-      <c r="P41" s="129"/>
-      <c r="Q41" s="129"/>
-      <c r="R41" s="129"/>
-      <c r="S41" s="129"/>
-      <c r="T41" s="129"/>
-      <c r="U41" s="129"/>
-      <c r="V41" s="129"/>
-      <c r="W41" s="129"/>
-      <c r="X41" s="129"/>
+      <c r="H41" s="125"/>
+      <c r="I41" s="125"/>
+      <c r="J41" s="125"/>
+      <c r="K41" s="125"/>
+      <c r="L41" s="125"/>
+      <c r="M41" s="125"/>
+      <c r="N41" s="125"/>
+      <c r="O41" s="125"/>
+      <c r="P41" s="125"/>
+      <c r="Q41" s="125"/>
+      <c r="R41" s="125"/>
+      <c r="S41" s="125"/>
+      <c r="T41" s="125"/>
+      <c r="U41" s="125"/>
+      <c r="V41" s="125"/>
+      <c r="W41" s="125"/>
+      <c r="X41" s="125"/>
       <c r="Y41" s="9"/>
     </row>
     <row r="42" spans="1:25" s="7" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4715,23 +4715,23 @@
       <c r="E43" s="9"/>
       <c r="F43" s="10"/>
       <c r="G43" s="10"/>
-      <c r="H43" s="129"/>
-      <c r="I43" s="129"/>
-      <c r="J43" s="129"/>
-      <c r="K43" s="129"/>
-      <c r="L43" s="129"/>
-      <c r="M43" s="129"/>
-      <c r="N43" s="129"/>
-      <c r="O43" s="129"/>
-      <c r="P43" s="129"/>
-      <c r="Q43" s="129"/>
-      <c r="R43" s="129"/>
-      <c r="S43" s="129"/>
-      <c r="T43" s="129"/>
-      <c r="U43" s="129"/>
-      <c r="V43" s="129"/>
-      <c r="W43" s="129"/>
-      <c r="X43" s="129"/>
+      <c r="H43" s="125"/>
+      <c r="I43" s="125"/>
+      <c r="J43" s="125"/>
+      <c r="K43" s="125"/>
+      <c r="L43" s="125"/>
+      <c r="M43" s="125"/>
+      <c r="N43" s="125"/>
+      <c r="O43" s="125"/>
+      <c r="P43" s="125"/>
+      <c r="Q43" s="125"/>
+      <c r="R43" s="125"/>
+      <c r="S43" s="125"/>
+      <c r="T43" s="125"/>
+      <c r="U43" s="125"/>
+      <c r="V43" s="125"/>
+      <c r="W43" s="125"/>
+      <c r="X43" s="125"/>
       <c r="Y43" s="9"/>
     </row>
     <row r="44" spans="1:25" s="7" customFormat="1" ht="5.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4769,12 +4769,12 @@
       <c r="E45" s="9"/>
       <c r="F45" s="10"/>
       <c r="G45" s="10"/>
-      <c r="H45" s="124" t="s">
+      <c r="H45" s="127" t="s">
         <v>396</v>
       </c>
-      <c r="I45" s="124"/>
-      <c r="J45" s="124"/>
-      <c r="K45" s="124"/>
+      <c r="I45" s="127"/>
+      <c r="J45" s="127"/>
+      <c r="K45" s="127"/>
       <c r="L45" s="19"/>
       <c r="M45" s="19"/>
       <c r="N45" s="19"/>
@@ -4784,10 +4784,10 @@
       <c r="R45" s="19"/>
       <c r="S45" s="19"/>
       <c r="T45" s="19"/>
-      <c r="U45" s="125" t="s">
+      <c r="U45" s="128" t="s">
         <v>397</v>
       </c>
-      <c r="V45" s="125"/>
+      <c r="V45" s="128"/>
       <c r="W45" s="19"/>
       <c r="X45" s="19"/>
       <c r="Y45" s="9"/>
@@ -4831,13 +4831,13 @@
       <c r="G47" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H47" s="129"/>
-      <c r="I47" s="129"/>
-      <c r="J47" s="129"/>
-      <c r="K47" s="129"/>
-      <c r="L47" s="129"/>
-      <c r="M47" s="129"/>
-      <c r="N47" s="129"/>
+      <c r="H47" s="125"/>
+      <c r="I47" s="125"/>
+      <c r="J47" s="125"/>
+      <c r="K47" s="125"/>
+      <c r="L47" s="125"/>
+      <c r="M47" s="125"/>
+      <c r="N47" s="125"/>
       <c r="O47" s="11"/>
       <c r="P47" s="11"/>
       <c r="Q47" s="11"/>
@@ -4889,16 +4889,16 @@
       <c r="G49" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H49" s="129"/>
-      <c r="I49" s="129"/>
-      <c r="J49" s="129"/>
-      <c r="K49" s="129"/>
-      <c r="L49" s="129"/>
-      <c r="M49" s="129"/>
-      <c r="N49" s="129"/>
-      <c r="O49" s="129"/>
-      <c r="P49" s="129"/>
-      <c r="Q49" s="129"/>
+      <c r="H49" s="125"/>
+      <c r="I49" s="125"/>
+      <c r="J49" s="125"/>
+      <c r="K49" s="125"/>
+      <c r="L49" s="125"/>
+      <c r="M49" s="125"/>
+      <c r="N49" s="125"/>
+      <c r="O49" s="125"/>
+      <c r="P49" s="125"/>
+      <c r="Q49" s="125"/>
       <c r="R49" s="11"/>
       <c r="S49" s="11"/>
       <c r="T49" s="11"/>
@@ -4947,15 +4947,15 @@
       <c r="G51" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H51" s="129"/>
-      <c r="I51" s="129"/>
-      <c r="J51" s="129"/>
-      <c r="K51" s="129"/>
-      <c r="L51" s="129"/>
-      <c r="M51" s="129"/>
-      <c r="N51" s="129"/>
-      <c r="O51" s="129"/>
-      <c r="P51" s="129"/>
+      <c r="H51" s="125"/>
+      <c r="I51" s="125"/>
+      <c r="J51" s="125"/>
+      <c r="K51" s="125"/>
+      <c r="L51" s="125"/>
+      <c r="M51" s="125"/>
+      <c r="N51" s="125"/>
+      <c r="O51" s="125"/>
+      <c r="P51" s="125"/>
       <c r="Q51" s="11"/>
       <c r="R51" s="11"/>
       <c r="S51" s="11"/>
@@ -5130,12 +5130,12 @@
       <c r="R57" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="S57" s="129"/>
-      <c r="T57" s="129"/>
-      <c r="U57" s="129"/>
-      <c r="V57" s="129"/>
-      <c r="W57" s="129"/>
-      <c r="X57" s="129"/>
+      <c r="S57" s="125"/>
+      <c r="T57" s="125"/>
+      <c r="U57" s="125"/>
+      <c r="V57" s="125"/>
+      <c r="W57" s="125"/>
+      <c r="X57" s="125"/>
       <c r="Y57" s="9"/>
     </row>
     <row r="58" spans="1:25" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5190,9 +5190,9 @@
       <c r="R59" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="S59" s="133"/>
-      <c r="T59" s="133"/>
-      <c r="U59" s="133"/>
+      <c r="S59" s="126"/>
+      <c r="T59" s="126"/>
+      <c r="U59" s="126"/>
       <c r="V59" s="2"/>
       <c r="W59" s="2"/>
       <c r="X59" s="2"/>
@@ -5206,10 +5206,10 @@
       <c r="C60" s="15" t="s">
         <v>405</v>
       </c>
-      <c r="D60" s="132">
+      <c r="D60" s="124">
         <v>20200131</v>
       </c>
-      <c r="E60" s="132"/>
+      <c r="E60" s="124"/>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -5266,12 +5266,6 @@
     <protectedRange sqref="H5:I5 H31:I31" name="Nama PT"/>
   </protectedRanges>
   <mergeCells count="19">
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="H47:N47"/>
-    <mergeCell ref="H49:Q49"/>
-    <mergeCell ref="H51:P51"/>
-    <mergeCell ref="S57:X57"/>
-    <mergeCell ref="S59:U59"/>
     <mergeCell ref="H45:K45"/>
     <mergeCell ref="U45:V45"/>
     <mergeCell ref="A2:Y2"/>
@@ -5285,6 +5279,12 @@
     <mergeCell ref="H33:X33"/>
     <mergeCell ref="H41:X41"/>
     <mergeCell ref="H43:X43"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="H47:N47"/>
+    <mergeCell ref="H49:Q49"/>
+    <mergeCell ref="H51:P51"/>
+    <mergeCell ref="S57:X57"/>
+    <mergeCell ref="S59:U59"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H17:J17" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -5574,9 +5574,9 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="153"/>
-      <c r="B8" s="153"/>
-      <c r="C8" s="153"/>
+      <c r="A8" s="154"/>
+      <c r="B8" s="154"/>
+      <c r="C8" s="154"/>
       <c r="D8" s="136" t="s">
         <v>69</v>
       </c>
@@ -5591,8 +5591,8 @@
       <c r="I8" s="134" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="153"/>
-      <c r="K8" s="153"/>
+      <c r="J8" s="154"/>
+      <c r="K8" s="154"/>
     </row>
     <row r="9" spans="1:12" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="135"/>
@@ -5679,17 +5679,17 @@
       <c r="K12" s="25"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="154" t="s">
+      <c r="A13" s="153" t="s">
         <v>428</v>
       </c>
-      <c r="B13" s="154"/>
-      <c r="C13" s="154"/>
-      <c r="D13" s="154"/>
-      <c r="E13" s="154"/>
-      <c r="F13" s="154"/>
-      <c r="G13" s="154"/>
-      <c r="H13" s="154"/>
-      <c r="I13" s="154"/>
+      <c r="B13" s="153"/>
+      <c r="C13" s="153"/>
+      <c r="D13" s="153"/>
+      <c r="E13" s="153"/>
+      <c r="F13" s="153"/>
+      <c r="G13" s="153"/>
+      <c r="H13" s="153"/>
+      <c r="I13" s="153"/>
       <c r="J13" s="80" t="e">
         <f>AVERAGE(J11:J12)</f>
         <v>#DIV/0!</v>
@@ -5700,17 +5700,17 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="154" t="s">
+      <c r="A14" s="153" t="s">
         <v>429</v>
       </c>
-      <c r="B14" s="154"/>
-      <c r="C14" s="154"/>
-      <c r="D14" s="154"/>
-      <c r="E14" s="154"/>
-      <c r="F14" s="154"/>
-      <c r="G14" s="154"/>
-      <c r="H14" s="154"/>
-      <c r="I14" s="154"/>
+      <c r="B14" s="153"/>
+      <c r="C14" s="153"/>
+      <c r="D14" s="153"/>
+      <c r="E14" s="153"/>
+      <c r="F14" s="153"/>
+      <c r="G14" s="153"/>
+      <c r="H14" s="153"/>
+      <c r="I14" s="153"/>
       <c r="J14" s="80" t="e">
         <f>AVERAGEIFS(J11:J12,C11:C12,"V")</f>
         <v>#DIV/0!</v>
@@ -5722,18 +5722,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="I8:I9"/>
     <mergeCell ref="A13:I13"/>
     <mergeCell ref="A14:I14"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="D7:I7"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="I8:I9"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C12" xr:uid="{00000000-0002-0000-0A00-000000000000}">
@@ -9103,7 +9103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
@@ -10227,6 +10227,199 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="L1" sqref="L1"/>
+      <selection pane="topRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20" style="3" customWidth="1"/>
+    <col min="3" max="6" width="9.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>163</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="38"/>
+    </row>
+    <row r="3" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="159" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="159" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="177" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="178"/>
+      <c r="E3" s="178"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="159" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="160"/>
+      <c r="B4" s="160"/>
+      <c r="C4" s="72" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="48" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="G4" s="160"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
+        <v>1</v>
+      </c>
+      <c r="B5" s="22">
+        <v>2</v>
+      </c>
+      <c r="C5" s="22">
+        <v>3</v>
+      </c>
+      <c r="D5" s="22">
+        <v>4</v>
+      </c>
+      <c r="E5" s="22">
+        <v>5</v>
+      </c>
+      <c r="F5" s="22">
+        <v>6</v>
+      </c>
+      <c r="G5" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
+        <v>1</v>
+      </c>
+      <c r="B6" s="49" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:8" ht="102" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <v>2</v>
+      </c>
+      <c r="B7" s="49" t="s">
+        <v>172</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <v>3</v>
+      </c>
+      <c r="B8" s="49" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
+        <v>4</v>
+      </c>
+      <c r="B9" s="49" t="s">
+        <v>174</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="31">
+        <v>5</v>
+      </c>
+      <c r="B10" s="49" t="s">
+        <v>175</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="180" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="181"/>
+      <c r="C11" s="73">
+        <f>SUM(C6:C10)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="73">
+        <f t="shared" ref="D11:F11" si="0">SUM(D6:D10)</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="73">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="73">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="74"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="A11:B11"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -10330,8 +10523,8 @@
       <c r="A8" s="142" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="181"/>
-      <c r="C8" s="181"/>
+      <c r="B8" s="176"/>
+      <c r="C8" s="176"/>
       <c r="D8" s="143"/>
       <c r="E8" s="25">
         <f>COUNTIF(E6:E7,"*")</f>
@@ -10350,7 +10543,294 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" customWidth="1"/>
+    <col min="2" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="134" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="134" t="s">
+        <v>283</v>
+      </c>
+      <c r="C14" s="134" t="s">
+        <v>284</v>
+      </c>
+      <c r="D14" s="136" t="s">
+        <v>285</v>
+      </c>
+      <c r="E14" s="137"/>
+      <c r="F14" s="138"/>
+      <c r="G14" s="134" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="135"/>
+      <c r="B15" s="135"/>
+      <c r="C15" s="135"/>
+      <c r="D15" s="84" t="s">
+        <v>287</v>
+      </c>
+      <c r="E15" s="84" t="s">
+        <v>288</v>
+      </c>
+      <c r="F15" s="84" t="s">
+        <v>289</v>
+      </c>
+      <c r="G15" s="135"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="29">
+        <v>1</v>
+      </c>
+      <c r="B16" s="29">
+        <v>2</v>
+      </c>
+      <c r="C16" s="29">
+        <v>2</v>
+      </c>
+      <c r="D16" s="29">
+        <v>3</v>
+      </c>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29">
+        <v>4</v>
+      </c>
+      <c r="G16" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="31">
+        <v>1</v>
+      </c>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="31">
+        <v>2</v>
+      </c>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="31">
+        <v>3</v>
+      </c>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="31">
+        <v>4</v>
+      </c>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="31">
+        <v>5</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="G14:G15"/>
+  </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D21" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>$B$4:$B$12</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="H1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -10454,8 +10934,8 @@
       <c r="A8" s="142" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="181"/>
-      <c r="C8" s="181"/>
+      <c r="B8" s="176"/>
+      <c r="C8" s="176"/>
       <c r="D8" s="143"/>
       <c r="E8" s="25">
         <f>COUNTIF(E6:E7,"*")</f>
@@ -10474,294 +10954,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:H21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.5703125" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1"/>
-    <col min="5" max="7" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="134" t="s">
-        <v>115</v>
-      </c>
-      <c r="B14" s="134" t="s">
-        <v>283</v>
-      </c>
-      <c r="C14" s="134" t="s">
-        <v>284</v>
-      </c>
-      <c r="D14" s="136" t="s">
-        <v>285</v>
-      </c>
-      <c r="E14" s="137"/>
-      <c r="F14" s="138"/>
-      <c r="G14" s="134" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="135"/>
-      <c r="B15" s="135"/>
-      <c r="C15" s="135"/>
-      <c r="D15" s="84" t="s">
-        <v>287</v>
-      </c>
-      <c r="E15" s="84" t="s">
-        <v>288</v>
-      </c>
-      <c r="F15" s="84" t="s">
-        <v>289</v>
-      </c>
-      <c r="G15" s="135"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
-        <v>1</v>
-      </c>
-      <c r="B16" s="29">
-        <v>2</v>
-      </c>
-      <c r="C16" s="29">
-        <v>2</v>
-      </c>
-      <c r="D16" s="29">
-        <v>3</v>
-      </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29">
-        <v>4</v>
-      </c>
-      <c r="G16" s="29">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="31">
-        <v>1</v>
-      </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="31">
-        <v>2</v>
-      </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="31">
-        <v>3</v>
-      </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="31">
-        <v>4</v>
-      </c>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="31">
-        <v>5</v>
-      </c>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="G14:G15"/>
-  </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D21" xr:uid="{00000000-0002-0000-0200-000000000000}">
-      <formula1>$B$4:$B$12</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="H1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -10865,8 +11058,8 @@
       <c r="A8" s="142" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="181"/>
-      <c r="C8" s="181"/>
+      <c r="B8" s="176"/>
+      <c r="C8" s="176"/>
       <c r="D8" s="143"/>
       <c r="E8" s="25">
         <f>COUNTIF(E6:E7,"*")</f>
@@ -10886,7 +11079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -11013,199 +11206,6 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-1F00-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="L1" sqref="L1"/>
-      <selection pane="topRight" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="5.5703125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="20" style="3" customWidth="1"/>
-    <col min="3" max="6" width="9.5703125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="23.140625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-    </row>
-    <row r="3" spans="1:8" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="159" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="159" t="s">
-        <v>164</v>
-      </c>
-      <c r="C3" s="176" t="s">
-        <v>165</v>
-      </c>
-      <c r="D3" s="177"/>
-      <c r="E3" s="177"/>
-      <c r="F3" s="178"/>
-      <c r="G3" s="159" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="160"/>
-      <c r="B4" s="160"/>
-      <c r="C4" s="72" t="s">
-        <v>167</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>168</v>
-      </c>
-      <c r="E4" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="G4" s="160"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="22">
-        <v>1</v>
-      </c>
-      <c r="B5" s="22">
-        <v>2</v>
-      </c>
-      <c r="C5" s="22">
-        <v>3</v>
-      </c>
-      <c r="D5" s="22">
-        <v>4</v>
-      </c>
-      <c r="E5" s="22">
-        <v>5</v>
-      </c>
-      <c r="F5" s="22">
-        <v>6</v>
-      </c>
-      <c r="G5" s="22">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="76.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="31">
-        <v>1</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>171</v>
-      </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-    </row>
-    <row r="7" spans="1:8" ht="102" x14ac:dyDescent="0.25">
-      <c r="A7" s="31">
-        <v>2</v>
-      </c>
-      <c r="B7" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-    </row>
-    <row r="8" spans="1:8" ht="114.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="31">
-        <v>3</v>
-      </c>
-      <c r="B8" s="49" t="s">
-        <v>173</v>
-      </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-    </row>
-    <row r="9" spans="1:8" ht="89.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="31">
-        <v>4</v>
-      </c>
-      <c r="B9" s="49" t="s">
-        <v>174</v>
-      </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="31">
-        <v>5</v>
-      </c>
-      <c r="B10" s="49" t="s">
-        <v>175</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="179" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="180"/>
-      <c r="C11" s="73">
-        <f>SUM(C6:C10)</f>
-        <v>0</v>
-      </c>
-      <c r="D11" s="73">
-        <f t="shared" ref="D11:F11" si="0">SUM(D6:D10)</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="73">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="73">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="74"/>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="A11:B11"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="H1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11353,7 +11353,7 @@
       <c r="A12" s="142" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="181"/>
+      <c r="B12" s="176"/>
       <c r="C12" s="143"/>
       <c r="D12" s="25">
         <f>COUNTIF(D10:D11,"V")</f>
@@ -11548,7 +11548,7 @@
       <c r="A13" s="142" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="181"/>
+      <c r="B13" s="176"/>
       <c r="C13" s="143"/>
       <c r="D13" s="25">
         <f>COUNTIF(D11:D12,"V")</f>
@@ -12241,11 +12241,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
     <mergeCell ref="J12:J13"/>
     <mergeCell ref="K12:K13"/>
     <mergeCell ref="A21:A22"/>
@@ -12256,11 +12256,11 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:I12"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
@@ -14736,7 +14736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
@@ -15919,6 +15919,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="L11:L12"/>
     <mergeCell ref="M11:M12"/>
     <mergeCell ref="F11:F12"/>
@@ -15927,11 +15932,6 @@
     <mergeCell ref="I11:I12"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14:G15 L14:L15" xr:uid="{00000000-0002-0000-0800-000000000000}">

</xml_diff>

<commit_message>
perbaiki expor kuantitatif prodi
</commit_message>
<xml_diff>
--- a/common/required/kriteria9/aps/template/kuantitatif.xlsx
+++ b/common/required/kriteria9/aps/template/kuantitatif.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adryanev\Code\php\kriteria\common\required\kriteria9\aps\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{564164A0-FADB-43A9-B9C3-3AC43A920F6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE820773-D931-42F2-B102-918DBE9525CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="839" firstSheet="18" activeTab="47" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="839" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="68" r:id="rId1"/>
@@ -246,7 +246,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="430">
   <si>
     <t xml:space="preserve">:   </t>
   </si>
@@ -2445,7 +2445,7 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2986,6 +2986,12 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3482,8 +3488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y61"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:X5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA2" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5513,7 +5519,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5735,7 +5741,7 @@
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:I9"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11:C12" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>$B$4:$B$5</formula1>
     </dataValidation>
@@ -5756,7 +5762,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="J16" sqref="J16"/>
+      <selection pane="bottomRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5932,7 +5938,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:F15" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>$F$4:$F$9</formula1>
     </dataValidation>
@@ -7156,7 +7162,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8868,7 +8874,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8984,7 +8990,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9108,7 +9114,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9232,7 +9238,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9340,14 +9346,14 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9497,14 +9503,14 @@
       <c r="D8" s="65"/>
       <c r="E8" s="65"/>
       <c r="F8" s="66" t="e">
-        <f t="shared" ref="F8:F19" si="0">AVERAGE(C8:E8)</f>
+        <f t="shared" ref="F8:F20" si="0">AVERAGE(C8:E8)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="G8" s="65"/>
       <c r="H8" s="65"/>
       <c r="I8" s="65"/>
       <c r="J8" s="66" t="e">
-        <f t="shared" ref="J8:J19" si="1">AVERAGE(G8:I8)</f>
+        <f t="shared" ref="J8:J20" si="1">AVERAGE(G8:I8)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -9736,7 +9742,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="31">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B18" s="49" t="s">
         <v>142</v>
@@ -9757,52 +9763,91 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="168" t="s">
+      <c r="A19" s="183" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="168"/>
+      <c r="B19" s="184"/>
       <c r="C19" s="107">
         <f>SUM(C16:C18)</f>
         <v>0</v>
       </c>
       <c r="D19" s="107">
-        <f>SUM(D16:D18)</f>
+        <f t="shared" ref="D19:E19" si="2">SUM(D16:D18)</f>
         <v>0</v>
       </c>
       <c r="E19" s="107">
-        <f>SUM(E16:E18)</f>
-        <v>0</v>
-      </c>
-      <c r="F19" s="107">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="66">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G19" s="107">
-        <f>SUM(G16:G18)</f>
+        <f t="shared" ref="G19" si="3">SUM(G16:G18)</f>
         <v>0</v>
       </c>
       <c r="H19" s="107">
-        <f>SUM(H16:H18)</f>
+        <f t="shared" ref="H19" si="4">SUM(H16:H18)</f>
         <v>0</v>
       </c>
       <c r="I19" s="107">
-        <f>SUM(I16:I18)</f>
-        <v>0</v>
-      </c>
-      <c r="J19" s="107">
+        <f t="shared" ref="I19" si="5">SUM(I16:I18)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="66">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="168" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="168"/>
+      <c r="C20" s="107">
+        <f>SUM(C12,C15,C19)</f>
+        <v>0</v>
+      </c>
+      <c r="D20" s="107">
+        <f t="shared" ref="D20:J20" si="6">SUM(D12,D15,D19)</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="107">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="107">
+        <f>AVERAGE(F12,F15,F19)</f>
+        <v>0</v>
+      </c>
+      <c r="G20" s="107">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="107">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="107">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="107">
+        <f>AVERAGE(J12,J15,J19)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A19:B19"/>
+  <mergeCells count="8">
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K1" location="'Daftar Tabel'!A1" display="&lt;&lt;&lt; Daftar Tabel" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
@@ -9821,7 +9866,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10132,7 +10177,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="A7" sqref="A7:F10"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10963,7 +11008,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13149,7 +13194,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3:XFD3"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14127,7 +14172,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14235,7 +14280,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14358,7 +14403,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C9:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14480,7 +14525,7 @@
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14736,7 +14781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="6" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
       <selection pane="topRight" activeCell="L1" sqref="L1"/>
@@ -15070,7 +15115,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="11" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3:XFD3"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15279,7 +15324,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15688,7 +15733,7 @@
       <pane xSplit="1" ySplit="13" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="L16" sqref="L16"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>